<commit_message>
new backup not good
</commit_message>
<xml_diff>
--- a/תיעוד גרסאות.xlsx
+++ b/תיעוד גרסאות.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Project_A-esp32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEBC0D0-2599-4BE3-BA9C-BA44C0166A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD15165C-11B2-4ABA-9A2D-1A415E41980E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-5630" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>נוסף קוד מתורגם ל C++</t>
+  </si>
+  <si>
+    <t>גרסה לא טובה. משהו לא עובד בכרטיס זיכרון</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -162,6 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +449,7 @@
   <dimension ref="D1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -464,8 +468,12 @@
       </c>
     </row>
     <row r="3" spans="4:17" x14ac:dyDescent="0.3">
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
+      <c r="D3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>45235</v>
+      </c>
     </row>
     <row r="4" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D4" s="4"/>

</xml_diff>